<commit_message>
Update 2: Fixed test cases and completed TC1,2,3,4,5,6,7,10,11
</commit_message>
<xml_diff>
--- a/Class12/Class12Capstone/Test Cases/API Specific Tests and Results/TCAPI Results.xlsx
+++ b/Class12/Class12Capstone/Test Cases/API Specific Tests and Results/TCAPI Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
   <si>
     <t>AC1: Able to add new veteranian</t>
   </si>
@@ -172,28 +172,10 @@
     <t xml:space="preserve">1. De Cow                                  2. Just Cow                                3. Cow Pow </t>
   </si>
   <si>
-    <t>10. Change specialties "id"</t>
-  </si>
-  <si>
-    <t>12. Cick Send</t>
-  </si>
-  <si>
-    <t>Status: 400 Bad Request             Displays "Could not execute statement" on the Response Body tab</t>
-  </si>
-  <si>
-    <t>Status: 201 Created                                       Displayed the created data in JSON format on the Response Body tab</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
     <t>1. Moo                                         2. Cowdepow                           3. Austin</t>
-  </si>
-  <si>
-    <t>15. Change specialties "id"</t>
-  </si>
-  <si>
-    <t>16. Click Send</t>
   </si>
   <si>
     <t>P</t>
@@ -284,25 +266,106 @@
     <t>Input more than 30 characters for First Name</t>
   </si>
   <si>
-    <t>13. Insert firstName data between the quotes</t>
-  </si>
-  <si>
     <t>1.qwertyuiopasdfghjklzxcvbnmqwert                                  2.mnbvcxzlkjhgfdsapoiuytrewqmnbvc                                3.qazwsxedcrfvtgbyhnujmikolpqazws</t>
   </si>
   <si>
-    <t>14. Insert lastName data between the qoutes</t>
-  </si>
-  <si>
     <t>9. Insert firstName data between the qoutes</t>
   </si>
   <si>
     <t>Input more than 30 characters for Last Name</t>
   </si>
   <si>
-    <t>13. Insert firstName data between the qoutes</t>
-  </si>
-  <si>
     <t>Input less than 2 characters for Last Name</t>
+  </si>
+  <si>
+    <t>1. Create a new Request for POST with URL https://clinic.doveryai-no-proveryai.com/petclinic/api/vets/</t>
+  </si>
+  <si>
+    <t>Basic Auth type is selected</t>
+  </si>
+  <si>
+    <t>7. Copy paste the Body data script in the Body input area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open AC1TC10and11body.txt </t>
+  </si>
+  <si>
+    <t>JSON type is selected</t>
+  </si>
+  <si>
+    <t>12. Click on Test tab</t>
+  </si>
+  <si>
+    <t>Displays Test input area</t>
+  </si>
+  <si>
+    <t>13. Copy paste the tests script in the Test input area</t>
+  </si>
+  <si>
+    <t>Open AC1TC10and11TestScript.txt</t>
+  </si>
+  <si>
+    <t>14. Insert the same first name data in pm.expect(jsonData.firstName).to.eql("insert name here");</t>
+  </si>
+  <si>
+    <t>15. Insert the same last name data in pm.expect(jsonData.lastName).to.eql("insert name here");</t>
+  </si>
+  <si>
+    <t>16. Change the same specialties type id number data in  pm.expect(jsonData.specialties).to.eql([{id:0, name:''}]);</t>
+  </si>
+  <si>
+    <t>17. Cick Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status: 400 Bad Request             Displays "Could not execute statement" on the Response Body tab                                                                                                                                           Response Test tab:                                  Successful POST request: FAIL          Status code name has striing: FAIL Content-Type is present: PASS        Check if First Name is empty: FAIL   Respons value for First Name is the same as input: FAIL                         Check if Last Name is empty: FAIL    Respons value for Last Name is the same as input: FAIL                                 Check if Specialties Type is not selected: FAIL                            Respons value for Specialties type is the same as input: FAIL                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status: 201 Created                                     Displayed the created data in JSON format on the Response Body tab                                                                                     Response Test tab:                    Successful POST request: PASS          Status code name has striing: PASS Content-Type is present: PASS        Check if First Name is empty: FAIL   Respons value for First Name is the same as input: PASS                         Check if Last Name is empty: FAIL    Respons value for Last Name is the same as input: PASS                                 Check if Specialties Type is not selected: FAIL                                 Respons value for Specialties type is the same as input: PASS        </t>
+  </si>
+  <si>
+    <t>Results:                                AC1TC10a.jpg, AC1TC10aT.jpg for input no. 1                   AC1TC10b.jpg, AC1TC10bT.jpg for input no. 2                    AC1TC10c.jpg, AC1TC10cT.jpg for input no. 3</t>
+  </si>
+  <si>
+    <t>18. Click on Body tab</t>
+  </si>
+  <si>
+    <t>19. Insert firstName data between the quotes</t>
+  </si>
+  <si>
+    <t>20. Insert lastName data between the qoutes</t>
+  </si>
+  <si>
+    <t>21. Change specialties "id"</t>
+  </si>
+  <si>
+    <t>22. Click on Test tab</t>
+  </si>
+  <si>
+    <t>23. Insert the same first name data in pm.expect(jsonData.firstName).to.eql("insert name here");</t>
+  </si>
+  <si>
+    <t>24. Insert the same last name data in pm.expect(jsonData.lastName).to.eql("insert name here");</t>
+  </si>
+  <si>
+    <t>25. Change the same specialties type id number data in  pm.expect(jsonData.specialties).to.eql([{id:0, name:''}]);</t>
+  </si>
+  <si>
+    <t>26. Click Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status: 400 Bad Request             Displays "Could not execute statement" on the Response Body tab                                                                                                                                           Response Test tab:                    Successful POST request: FAIL          Status code name has striing: FAIL Content-Type is present: PASS        Check if First Name is empty: FAIL   Respons value for First Name is the same as input: FAIL                         Check if Last Name is empty: FAIL    Respons value for Last Name is the same as input: FAIL                                 Check if Specialties Type is not selected: FAIL                            Respons value for Specialties type is the same as input: FAIL                                  </t>
+  </si>
+  <si>
+    <t>Results:                                AC1TC10d.jpg, AC1TC10dT.jpg for input no. 1                   AC1TC10e.jpg, AC1TC10eT.jpg for input no. 2                    AC1TC10f.jpg, AC1TC10fT.jpg for input no. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status: 400 Bad Request             Displays "Could not execute statement" on the Response Body tab                                                                                                                                           Response Test tab:                    Successful POST request: FAIL          Status code name has striing: FAIL Content-Type is present: PASS       Check if First Name is empty: FAIL   Respons value for First Name is the same as input: FAIL                         Check if Last Name is empty: FAIL    Respons value for Last Name is the same as input: FAIL                                 Check if Specialties Type is not selected: FAIL                            Respons value for Specialties type is the same as input: FAIL                                  </t>
+  </si>
+  <si>
+    <t>Results:                                AC1TC11a.jpg, AC1TC11aT.jpg for input no. 1                   AC1TC11b.jpg, AC1TC11bT.jpg for input no. 2                    AC1TC11c.jpg, AC1TC11cT.jpg for input no. 3</t>
+  </si>
+  <si>
+    <t>Results:                                AC1TC11d.jpg, AC1TC11dT.jpg for input no. 1                   AC1TC11e.jpg, AC1TC11eT.jpg for input no. 2                    AC1TC11f.jpg, AC1TC11fT.jpg for input no. 3</t>
   </si>
 </sst>
 </file>
@@ -393,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -429,11 +492,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -465,6 +593,35 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,7 +975,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -838,13 +995,15 @@
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30.75" thickBot="1">
       <c r="A11" s="3" t="s">
@@ -857,7 +1016,9 @@
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="30.75" thickBot="1">
       <c r="A12" s="3"/>
@@ -865,10 +1026,14 @@
         <v>17</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1">
       <c r="A13" s="3"/>
@@ -905,15 +1070,17 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="45.75" thickBot="1">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="5"/>
@@ -926,17 +1093,21 @@
         <v>25</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="45.75" thickBot="1">
       <c r="A18" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>26</v>
@@ -949,7 +1120,7 @@
     <row r="19" spans="1:7" ht="45.75" thickBot="1">
       <c r="A19" s="3"/>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>27</v>
@@ -962,299 +1133,569 @@
     <row r="20" spans="1:7" ht="15.75" thickBot="1">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C20" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="60.75" thickBot="1">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1">
       <c r="A21" s="3"/>
       <c r="B21" s="6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="105.75" thickBot="1">
-      <c r="A22" s="11" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" ht="45.75" thickBot="1">
+        <v>51</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="75.75" thickBot="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="B23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="6"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:7" ht="75.75" thickBot="1">
       <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="4">
-        <v>5</v>
-      </c>
+      <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="60.75" thickBot="1">
-      <c r="A25" s="6"/>
+    <row r="25" spans="1:7" ht="90.75" thickBot="1">
+      <c r="A25" s="3"/>
       <c r="B25" s="6" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="75.75" thickBot="1">
-      <c r="A26" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" ht="315.75" thickBot="1">
+      <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A27" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A27" s="3"/>
       <c r="B27" s="6" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A28" s="3"/>
+      <c r="G27" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="105.75" thickBot="1">
+      <c r="A28" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
+    <row r="29" spans="1:7" ht="45.75" thickBot="1">
       <c r="A29" s="3"/>
       <c r="B29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="B30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1">
       <c r="A31" s="3"/>
       <c r="B31" s="6" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C31" s="6"/>
-      <c r="D31" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="45.75" thickBot="1">
+      <c r="D31" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="75.75" thickBot="1">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="30.75" thickBot="1">
+        <v>64</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" ht="75.75" thickBot="1">
       <c r="A33" s="3"/>
       <c r="B33" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="C33" s="6"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="45.75" thickBot="1">
+    <row r="34" spans="1:7" ht="90.75" thickBot="1">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="105.75" thickBot="1">
-      <c r="A35" s="11" t="s">
-        <v>49</v>
-      </c>
+    <row r="35" spans="1:7" ht="300.75" thickBot="1">
+      <c r="A35" s="6"/>
       <c r="B35" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A36" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="B36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="4">
-        <v>2</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" ht="60.75" thickBot="1">
-      <c r="A37" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A37" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="B37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45.75" thickBot="1">
+    </row>
+    <row r="38" spans="1:7" ht="30.75" thickBot="1">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A39" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="G38" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A39" s="3"/>
       <c r="B39" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="4">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" ht="60.75" thickBot="1">
-      <c r="A41" s="6"/>
+      <c r="B40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A41" s="3"/>
       <c r="B41" s="6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C41" s="6"/>
-      <c r="D41" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="D41" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A43" s="3"/>
+      <c r="B43" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" ht="105.75" thickBot="1">
+      <c r="A45" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="4">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" ht="90.75" thickBot="1">
+      <c r="A51" s="3"/>
+      <c r="B51" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:7" ht="300.75" thickBot="1">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="15"/>
+      <c r="F52" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A53" s="3"/>
+      <c r="B53" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A55" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="4">
+        <v>3</v>
+      </c>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A57" s="3"/>
+      <c r="B57" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A58" s="3"/>
+      <c r="B58" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+    </row>
+    <row r="59" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A59" s="3"/>
+      <c r="B59" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+    </row>
+    <row r="60" spans="1:7" ht="90.75" thickBot="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+    </row>
+    <row r="61" spans="1:7" ht="300.75" thickBot="1">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>